<commit_message>
Added feature to download article images
</commit_message>
<xml_diff>
--- a/excel_file.xlsx
+++ b/excel_file.xlsx
@@ -466,7 +466,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>48 minutes ago</t>
+          <t>1 hour ago</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -494,7 +494,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>58 minutes ago</t>
+          <t>1 hour ago</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">

</xml_diff>